<commit_message>
creating and testing the CPBC report to its fullest
</commit_message>
<xml_diff>
--- a/config/template_for_CPBC.xlsx
+++ b/config/template_for_CPBC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\ExcelWizard\ExcelWizard\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBD17856-D43B-4856-9297-2B17E649EB4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70240108-5AD1-4321-96A9-E2D5EB2FD935}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -20,146 +20,29 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="71">
   <si>
     <t>B10/20 - AgPlenus</t>
   </si>
   <si>
-    <t>B10/20 - AgPlenus.1</t>
-  </si>
-  <si>
-    <t>B10/20 - AgPlenus.2</t>
-  </si>
-  <si>
-    <t>B10/20 - AgPlenus.3</t>
-  </si>
-  <si>
-    <t>B10/20 - AgPlenus.4</t>
-  </si>
-  <si>
-    <t>B10/20 - AgPlenus.5</t>
-  </si>
-  <si>
     <t>B20/20 - Lavie- Bio</t>
   </si>
   <si>
-    <t>B20/20 - Lavie- Bio.1</t>
-  </si>
-  <si>
-    <t>B20/20 - Lavie- Bio.2</t>
-  </si>
-  <si>
-    <t>B20/20 - Lavie- Bio.3</t>
-  </si>
-  <si>
-    <t>B20/20 - Lavie- Bio.4</t>
-  </si>
-  <si>
-    <t>B20/20 - Lavie- Bio.5</t>
-  </si>
-  <si>
-    <t>B20/20 - Lavie- Bio.6</t>
-  </si>
-  <si>
-    <t>B20/20 - Lavie- Bio.7</t>
-  </si>
-  <si>
-    <t>B20/20 - Lavie- Bio.8</t>
-  </si>
-  <si>
     <t>B40/20 - CPB</t>
   </si>
   <si>
-    <t>B40/20 - CPB.1</t>
-  </si>
-  <si>
-    <t>B40/20 - CPB.2</t>
-  </si>
-  <si>
-    <t>B40/20 - CPB.3</t>
-  </si>
-  <si>
     <t>B70/20 - Biomica</t>
   </si>
   <si>
-    <t>B70/20 - Biomica.1</t>
-  </si>
-  <si>
-    <t>B70/20 - Biomica.2</t>
-  </si>
-  <si>
-    <t>B70/20 - Biomica.3</t>
-  </si>
-  <si>
-    <t>B70/20 - Biomica.4</t>
-  </si>
-  <si>
     <t>B74/20 - Canonic</t>
   </si>
   <si>
-    <t>B74/20 - Canonic.1</t>
-  </si>
-  <si>
-    <t>B74/20 - Canonic.2</t>
-  </si>
-  <si>
-    <t>B74/20 - Canonic.3</t>
-  </si>
-  <si>
-    <t>B74/20 - Canonic.4</t>
-  </si>
-  <si>
-    <t>B74/20 - Canonic.5</t>
-  </si>
-  <si>
     <t>B80/20 - PRoduct</t>
   </si>
   <si>
-    <t>B80/20 - PRoduct.1</t>
-  </si>
-  <si>
-    <t>B80/20 - PRoduct.2</t>
-  </si>
-  <si>
-    <t>B80/20 - PRoduct.3</t>
-  </si>
-  <si>
-    <t>B80/20 - PRoduct.4</t>
-  </si>
-  <si>
-    <t>B80/20 - PRoduct.5</t>
-  </si>
-  <si>
-    <t>B80/20 - PRoduct.6</t>
-  </si>
-  <si>
-    <t>B80/20 - PRoduct.7</t>
-  </si>
-  <si>
-    <t>B80/20 - PRoduct.8</t>
-  </si>
-  <si>
-    <t>B80/20 - PRoduct.9</t>
-  </si>
-  <si>
     <t>B72/20 - Casterra</t>
   </si>
   <si>
-    <t>B72/20 - Casterra.1</t>
-  </si>
-  <si>
-    <t>B72/20 - Casterra.2</t>
-  </si>
-  <si>
-    <t>B72/20 - Casterra.3</t>
-  </si>
-  <si>
-    <t>B72/20 - Casterra.4</t>
-  </si>
-  <si>
-    <t>B72/20 - Casterra.5</t>
-  </si>
-  <si>
     <t>Entry Type</t>
   </si>
   <si>
@@ -214,24 +97,15 @@
     <t>P145 - Corteva</t>
   </si>
   <si>
-    <t>P192 - LAV 321</t>
-  </si>
-  <si>
     <t>P19 - Yalos</t>
   </si>
   <si>
-    <t>P84 - New program</t>
-  </si>
-  <si>
     <t>P82 - ICL</t>
   </si>
   <si>
     <t>P86 - Product</t>
   </si>
   <si>
-    <t>P85 - Syngenta</t>
-  </si>
-  <si>
     <t>P87 - LAV311</t>
   </si>
   <si>
@@ -256,9 +130,6 @@
     <t>P251 - MRSA 50S2</t>
   </si>
   <si>
-    <t>P252 - Cancer Immun adjuvant2</t>
-  </si>
-  <si>
     <t>P258 - New Indication TBD</t>
   </si>
   <si>
@@ -322,9 +193,6 @@
     <t>P403 - Casterra RUN Generator</t>
   </si>
   <si>
-    <t xml:space="preserve">P404 - Casterra Developing new varieties </t>
-  </si>
-  <si>
     <t>P405 - Casterra Develop no RICIN lines</t>
   </si>
   <si>
@@ -337,23 +205,44 @@
     <t>P0 - Vacation / Sickness</t>
   </si>
   <si>
-    <t>Unnamed: 57</t>
-  </si>
-  <si>
-    <t>Unnamed: 58</t>
-  </si>
-  <si>
-    <t>New Project 1</t>
-  </si>
-  <si>
-    <t>New Project 2</t>
+    <t>P192-LAV 321</t>
+  </si>
+  <si>
+    <t>P84-New program</t>
+  </si>
+  <si>
+    <t>P85-Syngenta</t>
+  </si>
+  <si>
+    <t>P252 - Cancer Immun adjuvant</t>
+  </si>
+  <si>
+    <t>P255 - IBD</t>
+  </si>
+  <si>
+    <t>P165 - Verb Biotics</t>
+  </si>
+  <si>
+    <t>P404 - Casterra Developing New Varieties</t>
+  </si>
+  <si>
+    <t>P999 - General3</t>
+  </si>
+  <si>
+    <t>New project 1</t>
+  </si>
+  <si>
+    <t>New project 2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="167" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -363,22 +252,37 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="177"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="David"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="13">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCE5FF"/>
-        <bgColor rgb="FFCCE5FF"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -388,56 +292,50 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF1F89DF"/>
-        <bgColor rgb="FF1F89DF"/>
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFDF761F"/>
-        <bgColor rgb="FFDF761F"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF3C68A"/>
-        <bgColor rgb="FFF3C68A"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF6EEAF3"/>
-        <bgColor rgb="FF6EEAF3"/>
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF6EF396"/>
-        <bgColor rgb="FF6EF396"/>
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFE9F483"/>
-        <bgColor rgb="FFE9F483"/>
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF4AB3EE"/>
-        <bgColor rgb="FF4AB3EE"/>
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF55FE33"/>
-        <bgColor rgb="FF55FE33"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFC5CE6"/>
-        <bgColor rgb="FFFC5CE6"/>
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -465,26 +363,82 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Comma 2" xfId="2" xr:uid="{765E197C-F202-4079-9062-258D2D5F985F}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{DC17AE0F-D30E-4A4B-88C8-9043305ACF41}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -784,374 +738,386 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BK14"/>
+  <dimension ref="A1:BM14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="BL2" sqref="BL2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:63" x14ac:dyDescent="0.3">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="2" t="s">
+    <row r="1" spans="1:65" ht="42" x14ac:dyDescent="0.3">
+      <c r="A1" s="4"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="S1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="T1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="U1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="V1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="W1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="X1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="AC1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AF1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="AG1" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="AH1" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="AI1" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="AJ1" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="AK1" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="AL1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="AM1" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="AN1" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="AO1" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="AP1" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="AQ1" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="AR1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="AS1" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="AT1" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="AU1" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="AV1" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="AW1" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="AX1" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="AY1" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="AZ1" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="BA1" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="BB1" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="BC1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="BD1" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="BE1" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="BF1" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="BG1" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="BH1" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="BI1" s="13"/>
+      <c r="BJ1" s="13"/>
+      <c r="BK1" s="4"/>
+      <c r="BL1" s="4"/>
+      <c r="BM1" s="7"/>
+    </row>
+    <row r="2" spans="1:65" ht="84" x14ac:dyDescent="0.3">
+      <c r="A2" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="B2" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="C2" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="D2" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="E2" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="F2" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="G2" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="H2" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="AA1" s="4" t="s">
+      <c r="I2" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="AB1" s="4" t="s">
+      <c r="J2" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="AC1" s="4" t="s">
+      <c r="K2" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="AD1" s="4" t="s">
+      <c r="L2" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="AE1" s="5" t="s">
+      <c r="M2" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="AF1" s="5" t="s">
+      <c r="N2" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="AG1" s="5" t="s">
+      <c r="O2" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="AH1" s="5" t="s">
+      <c r="P2" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="AI1" s="5" t="s">
+      <c r="Q2" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="AJ1" s="6" t="s">
+      <c r="R2" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="S2" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="AK1" s="6" t="s">
+      <c r="T2" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="U2" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="AL1" s="6" t="s">
+      <c r="V2" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="W2" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="AM1" s="6" t="s">
+      <c r="X2" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="AN1" s="6" t="s">
+      <c r="Y2" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z2" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="AO1" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="AP1" s="7" t="s">
+      <c r="AA2" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB2" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="AQ1" s="7" t="s">
+      <c r="AC2" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="AR1" s="7" t="s">
+      <c r="AD2" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="AS1" s="7" t="s">
+      <c r="AE2" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="AT1" s="7" t="s">
+      <c r="AF2" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="AU1" s="7" t="s">
+      <c r="AG2" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="AV1" s="7" t="s">
+      <c r="AH2" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="AI2" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="AW1" s="7" t="s">
+      <c r="AJ2" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="AK2" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="AX1" s="7" t="s">
+      <c r="AL2" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="AY1" s="7" t="s">
+      <c r="AM2" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="AZ1" s="8" t="s">
+      <c r="AN2" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="BA1" s="8" t="s">
+      <c r="AO2" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="BB1" s="8" t="s">
+      <c r="AP2" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="BC1" s="8" t="s">
+      <c r="AQ2" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="BD1" s="8" t="s">
+      <c r="AR2" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="BE1" s="8" t="s">
+      <c r="AS2" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="BF1" s="9"/>
-      <c r="BG1" s="10"/>
-      <c r="BH1" s="1"/>
-      <c r="BI1" s="1"/>
-      <c r="BJ1" s="1"/>
-      <c r="BK1" s="1"/>
+      <c r="AT2" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="AU2" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="AV2" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="AW2" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="AX2" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="AY2" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="AZ2" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="BA2" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="BB2" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="BC2" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="BD2" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="BE2" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="BF2" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="BG2" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="BH2" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="BI2" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="BJ2" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="BK2" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="BL2" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="BM2" s="7"/>
     </row>
-    <row r="2" spans="1:63" x14ac:dyDescent="0.3">
-      <c r="A2" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="G2" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="H2" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="I2" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="J2" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="K2" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="L2" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="M2" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="N2" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="O2" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="P2" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q2" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="R2" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="S2" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="T2" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="U2" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="V2" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="W2" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="X2" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="Y2" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="Z2" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="AA2" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="AB2" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="AC2" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="AD2" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="AE2" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="AF2" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="AG2" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="AH2" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="AI2" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="AJ2" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="AK2" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="AL2" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="AM2" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="AN2" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="AO2" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="AP2" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="AQ2" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="AR2" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="AS2" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="AT2" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="AU2" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="AV2" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="AW2" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="AX2" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="AY2" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="AZ2" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="BA2" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="BB2" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="BC2" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="BD2" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="BE2" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="BF2" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="BG2" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="BH2" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="BI2" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="BJ2" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="BK2" s="11" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="3" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
@@ -1202,21 +1168,22 @@
       <c r="BG3" s="1"/>
       <c r="BH3" s="1"/>
       <c r="BI3" s="1"/>
-      <c r="BJ3" s="1"/>
-      <c r="BK3" s="1"/>
+      <c r="BJ3" s="19"/>
+      <c r="BK3" s="19"/>
+      <c r="BL3" s="19"/>
     </row>
-    <row r="4" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
@@ -1267,21 +1234,22 @@
       <c r="BG4" s="1"/>
       <c r="BH4" s="1"/>
       <c r="BI4" s="1"/>
-      <c r="BJ4" s="1"/>
-      <c r="BK4" s="1"/>
+      <c r="BJ4" s="19"/>
+      <c r="BK4" s="19"/>
+      <c r="BL4" s="19"/>
     </row>
-    <row r="5" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
@@ -1332,21 +1300,22 @@
       <c r="BG5" s="1"/>
       <c r="BH5" s="1"/>
       <c r="BI5" s="1"/>
-      <c r="BJ5" s="1"/>
-      <c r="BK5" s="1"/>
+      <c r="BJ5" s="19"/>
+      <c r="BK5" s="19"/>
+      <c r="BL5" s="19"/>
     </row>
-    <row r="6" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
@@ -1397,21 +1366,22 @@
       <c r="BG6" s="1"/>
       <c r="BH6" s="1"/>
       <c r="BI6" s="1"/>
-      <c r="BJ6" s="1"/>
-      <c r="BK6" s="1"/>
+      <c r="BJ6" s="19"/>
+      <c r="BK6" s="19"/>
+      <c r="BL6" s="19"/>
     </row>
-    <row r="7" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="12"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
@@ -1462,21 +1432,22 @@
       <c r="BG7" s="1"/>
       <c r="BH7" s="1"/>
       <c r="BI7" s="1"/>
-      <c r="BJ7" s="1"/>
-      <c r="BK7" s="1"/>
+      <c r="BJ7" s="19"/>
+      <c r="BK7" s="19"/>
+      <c r="BL7" s="19"/>
     </row>
-    <row r="8" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="12"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
@@ -1527,21 +1498,22 @@
       <c r="BG8" s="1"/>
       <c r="BH8" s="1"/>
       <c r="BI8" s="1"/>
-      <c r="BJ8" s="1"/>
-      <c r="BK8" s="1"/>
+      <c r="BJ8" s="19"/>
+      <c r="BK8" s="19"/>
+      <c r="BL8" s="19"/>
     </row>
-    <row r="9" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="12"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
@@ -1592,21 +1564,22 @@
       <c r="BG9" s="1"/>
       <c r="BH9" s="1"/>
       <c r="BI9" s="1"/>
-      <c r="BJ9" s="1"/>
-      <c r="BK9" s="1"/>
+      <c r="BJ9" s="19"/>
+      <c r="BK9" s="19"/>
+      <c r="BL9" s="19"/>
     </row>
-    <row r="10" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="12"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
@@ -1657,21 +1630,22 @@
       <c r="BG10" s="1"/>
       <c r="BH10" s="1"/>
       <c r="BI10" s="1"/>
-      <c r="BJ10" s="1"/>
-      <c r="BK10" s="1"/>
+      <c r="BJ10" s="19"/>
+      <c r="BK10" s="19"/>
+      <c r="BL10" s="19"/>
     </row>
-    <row r="11" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="12"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
@@ -1722,21 +1696,22 @@
       <c r="BG11" s="1"/>
       <c r="BH11" s="1"/>
       <c r="BI11" s="1"/>
-      <c r="BJ11" s="1"/>
-      <c r="BK11" s="1"/>
+      <c r="BJ11" s="19"/>
+      <c r="BK11" s="19"/>
+      <c r="BL11" s="19"/>
     </row>
-    <row r="12" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
-      <c r="K12" s="12"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
@@ -1787,21 +1762,22 @@
       <c r="BG12" s="1"/>
       <c r="BH12" s="1"/>
       <c r="BI12" s="1"/>
-      <c r="BJ12" s="1"/>
-      <c r="BK12" s="1"/>
+      <c r="BJ12" s="19"/>
+      <c r="BK12" s="19"/>
+      <c r="BL12" s="19"/>
     </row>
-    <row r="13" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="12"/>
-      <c r="K13" s="12"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
@@ -1852,21 +1828,22 @@
       <c r="BG13" s="1"/>
       <c r="BH13" s="1"/>
       <c r="BI13" s="1"/>
-      <c r="BJ13" s="1"/>
-      <c r="BK13" s="1"/>
+      <c r="BJ13" s="19"/>
+      <c r="BK13" s="19"/>
+      <c r="BL13" s="19"/>
     </row>
-    <row r="14" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="12"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
@@ -1917,8 +1894,9 @@
       <c r="BG14" s="1"/>
       <c r="BH14" s="1"/>
       <c r="BI14" s="1"/>
-      <c r="BJ14" s="1"/>
-      <c r="BK14" s="1"/>
+      <c r="BJ14" s="19"/>
+      <c r="BK14" s="19"/>
+      <c r="BL14" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
adding parsers to the script
</commit_message>
<xml_diff>
--- a/config/template_for_CPBC.xlsx
+++ b/config/template_for_CPBC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\ExcelWizard\ExcelWizard\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70240108-5AD1-4321-96A9-E2D5EB2FD935}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0615C33B-4FC3-4554-AA4B-3C7C36F6825B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -240,7 +240,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -277,7 +277,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -338,6 +338,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF66FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -366,7 +378,7 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -409,10 +421,6 @@
       <alignment wrapText="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection hidden="1"/>
@@ -429,11 +437,15 @@
       <alignment vertical="top" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma 2" xfId="2" xr:uid="{765E197C-F202-4079-9062-258D2D5F985F}"/>
@@ -442,6 +454,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF66FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -740,8 +757,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BM14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="BL2" sqref="BL2"/>
+    <sheetView tabSelected="1" topLeftCell="AY1" workbookViewId="0">
+      <selection activeCell="BJ1" sqref="BJ1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -905,203 +922,203 @@
       <c r="BH1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="BI1" s="13"/>
-      <c r="BJ1" s="13"/>
+      <c r="BI1" s="18"/>
+      <c r="BJ1" s="19"/>
       <c r="BK1" s="4"/>
       <c r="BL1" s="4"/>
       <c r="BM1" s="7"/>
     </row>
     <row r="2" spans="1:65" ht="84" x14ac:dyDescent="0.3">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="H2" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="14" t="s">
+      <c r="I2" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="14" t="s">
+      <c r="J2" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="K2" s="14" t="s">
+      <c r="K2" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="L2" s="15" t="s">
+      <c r="L2" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="M2" s="15" t="s">
+      <c r="M2" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="N2" s="15" t="s">
+      <c r="N2" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="O2" s="15" t="s">
+      <c r="O2" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="P2" s="16" t="s">
+      <c r="P2" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="Q2" s="15" t="s">
+      <c r="Q2" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="R2" s="15" t="s">
+      <c r="R2" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="S2" s="15" t="s">
+      <c r="S2" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="T2" s="15" t="s">
+      <c r="T2" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="U2" s="15" t="s">
+      <c r="U2" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="V2" s="15" t="s">
+      <c r="V2" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="W2" s="15" t="s">
+      <c r="W2" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="X2" s="15" t="s">
+      <c r="X2" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="Y2" s="15" t="s">
+      <c r="Y2" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="Z2" s="15" t="s">
+      <c r="Z2" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="AA2" s="15" t="s">
+      <c r="AA2" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="AB2" s="15" t="s">
+      <c r="AB2" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="AC2" s="15" t="s">
+      <c r="AC2" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="AD2" s="15" t="s">
+      <c r="AD2" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="AE2" s="15" t="s">
+      <c r="AE2" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="AF2" s="15" t="s">
+      <c r="AF2" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="AG2" s="15" t="s">
+      <c r="AG2" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="AH2" s="15" t="s">
+      <c r="AH2" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="AI2" s="15" t="s">
+      <c r="AI2" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="AJ2" s="15" t="s">
+      <c r="AJ2" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="AK2" s="15" t="s">
+      <c r="AK2" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="AL2" s="15" t="s">
+      <c r="AL2" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="AM2" s="15" t="s">
+      <c r="AM2" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="AN2" s="15" t="s">
+      <c r="AN2" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="AO2" s="15" t="s">
+      <c r="AO2" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="AP2" s="15" t="s">
+      <c r="AP2" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="AQ2" s="15" t="s">
+      <c r="AQ2" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="AR2" s="15" t="s">
+      <c r="AR2" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="AS2" s="15" t="s">
+      <c r="AS2" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="AT2" s="15" t="s">
+      <c r="AT2" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="AU2" s="15" t="s">
+      <c r="AU2" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="AV2" s="15" t="s">
+      <c r="AV2" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="AW2" s="15" t="s">
+      <c r="AW2" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="AX2" s="15" t="s">
+      <c r="AX2" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="AY2" s="15" t="s">
+      <c r="AY2" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="AZ2" s="15" t="s">
+      <c r="AZ2" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="BA2" s="15" t="s">
+      <c r="BA2" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="BB2" s="15" t="s">
+      <c r="BB2" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="BC2" s="15" t="s">
+      <c r="BC2" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="BD2" s="15" t="s">
+      <c r="BD2" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="BE2" s="15" t="s">
+      <c r="BE2" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="BF2" s="15" t="s">
+      <c r="BF2" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="BG2" s="17" t="s">
+      <c r="BG2" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="BH2" s="17" t="s">
+      <c r="BH2" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="BI2" s="18" t="s">
+      <c r="BI2" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="BJ2" s="18" t="s">
+      <c r="BJ2" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="BK2" s="18" t="s">
+      <c r="BK2" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="BL2" s="18" t="s">
+      <c r="BL2" s="16" t="s">
         <v>70</v>
       </c>
       <c r="BM2" s="7"/>
@@ -1168,9 +1185,9 @@
       <c r="BG3" s="1"/>
       <c r="BH3" s="1"/>
       <c r="BI3" s="1"/>
-      <c r="BJ3" s="19"/>
-      <c r="BK3" s="19"/>
-      <c r="BL3" s="19"/>
+      <c r="BJ3" s="17"/>
+      <c r="BK3" s="17"/>
+      <c r="BL3" s="17"/>
     </row>
     <row r="4" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
@@ -1234,9 +1251,9 @@
       <c r="BG4" s="1"/>
       <c r="BH4" s="1"/>
       <c r="BI4" s="1"/>
-      <c r="BJ4" s="19"/>
-      <c r="BK4" s="19"/>
-      <c r="BL4" s="19"/>
+      <c r="BJ4" s="17"/>
+      <c r="BK4" s="17"/>
+      <c r="BL4" s="17"/>
     </row>
     <row r="5" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
@@ -1300,9 +1317,9 @@
       <c r="BG5" s="1"/>
       <c r="BH5" s="1"/>
       <c r="BI5" s="1"/>
-      <c r="BJ5" s="19"/>
-      <c r="BK5" s="19"/>
-      <c r="BL5" s="19"/>
+      <c r="BJ5" s="17"/>
+      <c r="BK5" s="17"/>
+      <c r="BL5" s="17"/>
     </row>
     <row r="6" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
@@ -1366,9 +1383,9 @@
       <c r="BG6" s="1"/>
       <c r="BH6" s="1"/>
       <c r="BI6" s="1"/>
-      <c r="BJ6" s="19"/>
-      <c r="BK6" s="19"/>
-      <c r="BL6" s="19"/>
+      <c r="BJ6" s="17"/>
+      <c r="BK6" s="17"/>
+      <c r="BL6" s="17"/>
     </row>
     <row r="7" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
@@ -1432,9 +1449,9 @@
       <c r="BG7" s="1"/>
       <c r="BH7" s="1"/>
       <c r="BI7" s="1"/>
-      <c r="BJ7" s="19"/>
-      <c r="BK7" s="19"/>
-      <c r="BL7" s="19"/>
+      <c r="BJ7" s="17"/>
+      <c r="BK7" s="17"/>
+      <c r="BL7" s="17"/>
     </row>
     <row r="8" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
@@ -1498,9 +1515,9 @@
       <c r="BG8" s="1"/>
       <c r="BH8" s="1"/>
       <c r="BI8" s="1"/>
-      <c r="BJ8" s="19"/>
-      <c r="BK8" s="19"/>
-      <c r="BL8" s="19"/>
+      <c r="BJ8" s="17"/>
+      <c r="BK8" s="17"/>
+      <c r="BL8" s="17"/>
     </row>
     <row r="9" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
@@ -1564,9 +1581,9 @@
       <c r="BG9" s="1"/>
       <c r="BH9" s="1"/>
       <c r="BI9" s="1"/>
-      <c r="BJ9" s="19"/>
-      <c r="BK9" s="19"/>
-      <c r="BL9" s="19"/>
+      <c r="BJ9" s="17"/>
+      <c r="BK9" s="17"/>
+      <c r="BL9" s="17"/>
     </row>
     <row r="10" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
@@ -1630,9 +1647,9 @@
       <c r="BG10" s="1"/>
       <c r="BH10" s="1"/>
       <c r="BI10" s="1"/>
-      <c r="BJ10" s="19"/>
-      <c r="BK10" s="19"/>
-      <c r="BL10" s="19"/>
+      <c r="BJ10" s="17"/>
+      <c r="BK10" s="17"/>
+      <c r="BL10" s="17"/>
     </row>
     <row r="11" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
@@ -1696,9 +1713,9 @@
       <c r="BG11" s="1"/>
       <c r="BH11" s="1"/>
       <c r="BI11" s="1"/>
-      <c r="BJ11" s="19"/>
-      <c r="BK11" s="19"/>
-      <c r="BL11" s="19"/>
+      <c r="BJ11" s="17"/>
+      <c r="BK11" s="17"/>
+      <c r="BL11" s="17"/>
     </row>
     <row r="12" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
@@ -1762,9 +1779,9 @@
       <c r="BG12" s="1"/>
       <c r="BH12" s="1"/>
       <c r="BI12" s="1"/>
-      <c r="BJ12" s="19"/>
-      <c r="BK12" s="19"/>
-      <c r="BL12" s="19"/>
+      <c r="BJ12" s="17"/>
+      <c r="BK12" s="17"/>
+      <c r="BL12" s="17"/>
     </row>
     <row r="13" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
@@ -1828,9 +1845,9 @@
       <c r="BG13" s="1"/>
       <c r="BH13" s="1"/>
       <c r="BI13" s="1"/>
-      <c r="BJ13" s="19"/>
-      <c r="BK13" s="19"/>
-      <c r="BL13" s="19"/>
+      <c r="BJ13" s="17"/>
+      <c r="BK13" s="17"/>
+      <c r="BL13" s="17"/>
     </row>
     <row r="14" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
@@ -1894,9 +1911,9 @@
       <c r="BG14" s="1"/>
       <c r="BH14" s="1"/>
       <c r="BI14" s="1"/>
-      <c r="BJ14" s="19"/>
-      <c r="BK14" s="19"/>
-      <c r="BL14" s="19"/>
+      <c r="BJ14" s="17"/>
+      <c r="BK14" s="17"/>
+      <c r="BL14" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
fixing astetic bugs and making each script independet
</commit_message>
<xml_diff>
--- a/config/template_for_CPBC.xlsx
+++ b/config/template_for_CPBC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\ExcelWizard\ExcelWizard\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F6F779D-A5B5-4274-BC8B-F4939C1EF6EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FA4AEA2-E27D-4E4F-A6E8-FBD00F3D2AA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -235,9 +235,6 @@
     <t>P999 - General5</t>
   </si>
   <si>
-    <t>P252 - Cancer Immun adjuvant2</t>
-  </si>
-  <si>
     <t>P254 - IBS</t>
   </si>
   <si>
@@ -254,6 +251,9 @@
   </si>
   <si>
     <t>New project2</t>
+  </si>
+  <si>
+    <t>P252 - Cancer Immun adjuvant</t>
   </si>
 </sst>
 </file>
@@ -905,8 +905,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BS14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AE1" zoomScale="62" workbookViewId="0">
-      <selection activeCell="P19" sqref="P19"/>
+    <sheetView tabSelected="1" topLeftCell="AC2" zoomScale="150" workbookViewId="0">
+      <selection activeCell="AL3" sqref="AL3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1209,10 +1209,10 @@
         <v>35</v>
       </c>
       <c r="AL2" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="AM2" s="19" t="s">
         <v>71</v>
-      </c>
-      <c r="AM2" s="19" t="s">
-        <v>72</v>
       </c>
       <c r="AN2" s="19" t="s">
         <v>60</v>
@@ -1272,7 +1272,7 @@
         <v>61</v>
       </c>
       <c r="BG2" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="BH2" s="19" t="s">
         <v>53</v>
@@ -1287,10 +1287,10 @@
         <v>56</v>
       </c>
       <c r="BL2" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="BM2" s="19" t="s">
         <v>74</v>
-      </c>
-      <c r="BM2" s="19" t="s">
-        <v>75</v>
       </c>
       <c r="BN2" s="19" t="s">
         <v>57</v>
@@ -1305,10 +1305,10 @@
         <v>64</v>
       </c>
       <c r="BR2" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="BS2" s="23" t="s">
         <v>76</v>
-      </c>
-      <c r="BS2" s="23" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:71" x14ac:dyDescent="0.3">

</xml_diff>